<commit_message>
Update drawing book, ME plan, and MEL
</commit_message>
<xml_diff>
--- a/mechanical/Drawings/Fox_Plus_DrawingBook.xlsx
+++ b/mechanical/Drawings/Fox_Plus_DrawingBook.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arobi\Documents\Repos\fox-plus\mechanical\Drawings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D934D311-0C64-47C5-ADCC-7EFDA6CE65B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B67BAA-C8E1-44D2-901B-18374368F5DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="450" windowWidth="26475" windowHeight="15300" xr2:uid="{C06F8B60-55CC-498C-8AD9-8EBD498CFFE4}"/>
+    <workbookView xWindow="1005" yWindow="225" windowWidth="26475" windowHeight="15300" activeTab="3" xr2:uid="{C06F8B60-55CC-498C-8AD9-8EBD498CFFE4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ED" sheetId="2" r:id="rId1"/>
+    <sheet name="ME" sheetId="1" r:id="rId2"/>
+    <sheet name="ML" sheetId="3" r:id="rId3"/>
+    <sheet name="PN" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>Drawing  #</t>
   </si>
@@ -51,94 +54,145 @@
     <t>Fox Plus Drawing Book</t>
   </si>
   <si>
-    <t>FP-ME-0001</t>
-  </si>
-  <si>
-    <t>FP-ME-0002</t>
-  </si>
-  <si>
-    <t>FP-ME-0003</t>
-  </si>
-  <si>
-    <t>FP-ME-0004</t>
-  </si>
-  <si>
-    <t>FP-ME-0005</t>
-  </si>
-  <si>
-    <t>FP-ME-0006</t>
-  </si>
-  <si>
-    <t>FP-ME-0007</t>
-  </si>
-  <si>
-    <t>FP-ME-0008</t>
-  </si>
-  <si>
-    <t>FP-ME-0009</t>
-  </si>
-  <si>
-    <t>FP-ME-0010</t>
-  </si>
-  <si>
-    <t>FP-ME-0011</t>
-  </si>
-  <si>
-    <t>FP-ME-0012</t>
-  </si>
-  <si>
-    <t>FP-ME-0013</t>
-  </si>
-  <si>
-    <t>FP-ME-0014</t>
-  </si>
-  <si>
-    <t>FP-ME-0015</t>
-  </si>
-  <si>
-    <t>FP-ME-0016</t>
-  </si>
-  <si>
-    <t>FP-ME-0017</t>
-  </si>
-  <si>
-    <t>FP-ME-0018</t>
-  </si>
-  <si>
-    <t>FP-ME-0019</t>
-  </si>
-  <si>
-    <t>FP-ME-0020</t>
-  </si>
-  <si>
-    <t>FP-ME-0021</t>
-  </si>
-  <si>
-    <t>FP-ME-0022</t>
-  </si>
-  <si>
-    <t>FP-ME-0023</t>
-  </si>
-  <si>
-    <t>FP-ME-0024</t>
-  </si>
-  <si>
-    <t>FP-ME-0025</t>
-  </si>
-  <si>
-    <t>FP-ME-0026</t>
-  </si>
-  <si>
-    <t>FP-ME-0027</t>
-  </si>
-  <si>
-    <t>FP-ME-0028</t>
-  </si>
-  <si>
-    <t>FP-ME-0029</t>
-  </si>
-  <si>
-    <t>FP-ME-0030</t>
+    <t>ME: Mechanical Drawings</t>
+  </si>
+  <si>
+    <t>ED: Engineering Data</t>
+  </si>
+  <si>
+    <t>FP-ED-001</t>
+  </si>
+  <si>
+    <t>FP-ED-002</t>
+  </si>
+  <si>
+    <t>FP-ED-003</t>
+  </si>
+  <si>
+    <t>FP-ED-004</t>
+  </si>
+  <si>
+    <t>FP-ED-005</t>
+  </si>
+  <si>
+    <t>FP-ED-006</t>
+  </si>
+  <si>
+    <t>FP-ED-007</t>
+  </si>
+  <si>
+    <t>FP-ED-008</t>
+  </si>
+  <si>
+    <t>FP-ED-009</t>
+  </si>
+  <si>
+    <t>FP-ED-010</t>
+  </si>
+  <si>
+    <t>FP-ME-001</t>
+  </si>
+  <si>
+    <t>FP-ME-002</t>
+  </si>
+  <si>
+    <t>FP-ME-003</t>
+  </si>
+  <si>
+    <t>FP-ME-004</t>
+  </si>
+  <si>
+    <t>FP-ME-005</t>
+  </si>
+  <si>
+    <t>FP-ME-006</t>
+  </si>
+  <si>
+    <t>FP-ME-007</t>
+  </si>
+  <si>
+    <t>FP-ME-008</t>
+  </si>
+  <si>
+    <t>FP-ME-009</t>
+  </si>
+  <si>
+    <t>FP-ME-010</t>
+  </si>
+  <si>
+    <t>ML: Parts Lists</t>
+  </si>
+  <si>
+    <t>FP-ML-001</t>
+  </si>
+  <si>
+    <t>FP-ML-002</t>
+  </si>
+  <si>
+    <t>FP-ML-003</t>
+  </si>
+  <si>
+    <t>FP-ML-004</t>
+  </si>
+  <si>
+    <t>FP-ML-005</t>
+  </si>
+  <si>
+    <t>FP-ML-006</t>
+  </si>
+  <si>
+    <t>FP-ML-007</t>
+  </si>
+  <si>
+    <t>FP-ML-008</t>
+  </si>
+  <si>
+    <t>FP-ML-009</t>
+  </si>
+  <si>
+    <t>FP-ML-010</t>
+  </si>
+  <si>
+    <t>Fox+ Major Equipment List (MEL)</t>
+  </si>
+  <si>
+    <t>A Robinson</t>
+  </si>
+  <si>
+    <t>PN: Plans</t>
+  </si>
+  <si>
+    <t>FP-PN-001</t>
+  </si>
+  <si>
+    <t>FP-PN-002</t>
+  </si>
+  <si>
+    <t>FP-PN-003</t>
+  </si>
+  <si>
+    <t>FP-PN-004</t>
+  </si>
+  <si>
+    <t>FP-PN-005</t>
+  </si>
+  <si>
+    <t>FP-PN-006</t>
+  </si>
+  <si>
+    <t>FP-PN-007</t>
+  </si>
+  <si>
+    <t>FP-PN-008</t>
+  </si>
+  <si>
+    <t>FP-PN-009</t>
+  </si>
+  <si>
+    <t>FP-PN-010</t>
+  </si>
+  <si>
+    <t>Fox+ Space Vehicle Mechanical Plan</t>
   </si>
 </sst>
 </file>
@@ -546,11 +600,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE6B1BE-5B34-474F-A6EB-0CF2EA30C1BB}">
-  <dimension ref="A1:M83"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A6C5165-52C9-4D01-AD3F-C388E03FC19C}">
+  <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,40 +620,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="2" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="6"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="2"/>
@@ -607,7 +658,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="2"/>
@@ -615,7 +666,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="2"/>
@@ -623,7 +674,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="2"/>
@@ -631,7 +682,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="2"/>
@@ -639,7 +690,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="2"/>
@@ -647,15 +698,15 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="2"/>
@@ -663,7 +714,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="2"/>
@@ -671,235 +722,178 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
       <c r="B15" s="3"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
       <c r="B16" s="3"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="7"/>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="9"/>
+    <row r="21" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="7"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="3"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="9"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>24</v>
-      </c>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="8"/>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="3"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="3"/>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>29</v>
-      </c>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="3"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>30</v>
-      </c>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>31</v>
-      </c>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="3"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>32</v>
-      </c>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>33</v>
-      </c>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="3"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>34</v>
-      </c>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="3"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="3"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="3"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="3"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="3"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="3"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="3"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="3"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="3"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="3"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="3"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="3"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="3"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -1078,6 +1072,1477 @@
       <c r="B83" s="3"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B84" s="3"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE6B1BE-5B34-474F-A6EB-0CF2EA30C1BB}">
+  <dimension ref="A1:M84"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="7"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="9"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="3"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="3"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="3"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="3"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="3"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="3"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="3"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="3"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="3"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="3"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="3"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="3"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="3"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="3"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="3"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="3"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="3"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="3"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="3"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="3"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="3"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="3"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="3"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="3"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="3"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="3"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="3"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="3"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="3"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="3"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="3"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="3"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62" s="3"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="3"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="3"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="3"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="3"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="3"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="3"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="3"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="3"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="3"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="3"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="3"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="3"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="3"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="3"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="3"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="3"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="3"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="3"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="3"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="3"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="3"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B84" s="3"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6497F1D6-3F8E-4451-BBB0-E93E9F4DE79B}">
+  <dimension ref="A1:M84"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="7"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="9"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="3"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="3"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="3"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="3"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="3"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="3"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="3"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="3"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="3"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="3"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="3"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="3"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="3"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="3"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="3"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="3"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="3"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="3"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="3"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="3"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="3"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="3"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="3"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="3"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="3"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="3"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="3"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="3"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="3"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="3"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="3"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="3"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62" s="3"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="3"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="3"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="3"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="3"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="3"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="3"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="3"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="3"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="3"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="3"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="3"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="3"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="3"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="3"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="3"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="3"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="3"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="3"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="3"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="3"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="3"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B84" s="3"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C9B4B11-B911-444B-B881-7398021D206F}">
+  <dimension ref="A1:M84"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="7"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="9"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="3"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="3"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="3"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="3"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="3"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="3"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="3"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="3"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="3"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="3"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="3"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="3"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="3"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="3"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="3"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="3"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="3"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="3"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="3"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="3"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="3"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="3"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="3"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="3"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="3"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="3"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="3"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="3"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="3"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="3"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="3"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="3"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62" s="3"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="3"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="3"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="3"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="3"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="3"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="3"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="3"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="3"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="3"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="3"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="3"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="3"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="3"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="3"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="3"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="3"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="3"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="3"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="3"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="3"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="3"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B84" s="3"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>